<commit_message>
Files related to agreement (last modified Dec. 9th, 2019)
</commit_message>
<xml_diff>
--- a/resources/agreement.xlsx
+++ b/resources/agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/db-mining/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/Workspace/db-mining/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF751978-4DDD-A24E-A903-312E41B3A1BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DACD6B2-AEFF-584C-AA11-F1642C4D5C10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9F3891A7-3AB5-7A4E-AF5F-D9A70803E654}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{9F3891A7-3AB5-7A4E-AF5F-D9A70803E654}"/>
   </bookViews>
   <sheets>
     <sheet name="Round1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>EXECUTION_ID</t>
   </si>
@@ -70,6 +73,15 @@
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>GABARITO</t>
+  </si>
+  <si>
+    <t>VANESSA</t>
+  </si>
+  <si>
+    <t>LEO</t>
   </si>
 </sst>
 </file>
@@ -139,7 +151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,6 +170,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,19 +486,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37769CC-B00B-9D42-9668-5184DBCA9DEC}">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J1" sqref="J1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,8 +512,20 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3029</v>
       </c>
@@ -520,8 +546,22 @@
       <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>3029</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <f>C2=K2</f>
+        <v>1</v>
+      </c>
+      <c r="M2" t="b">
+        <f>B2=K2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3035</v>
       </c>
@@ -546,8 +586,22 @@
         <f>COUNTIF(D:D,"DIFF_1_0")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>3035</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <f t="shared" ref="L3:L66" si="1">C3=K3</f>
+        <v>1</v>
+      </c>
+      <c r="M3" t="b">
+        <f t="shared" ref="M3:M66" si="2">B3=K3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3059</v>
       </c>
@@ -572,8 +626,22 @@
         <f>COUNTIF(D:D,"SAME_0")</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>3059</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M4" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3062</v>
       </c>
@@ -587,8 +655,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>3062</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M5" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3074</v>
       </c>
@@ -609,8 +691,22 @@
         <f>(G3+H4)/(G3+H3+G4+H4)</f>
         <v>0.87</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>3074</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3148</v>
       </c>
@@ -631,8 +727,22 @@
         <f>((G3+H3)/(G3+H3+G4+H4))*((G3+G4)/(G3+H3+G4+H4))</f>
         <v>7.1400000000000005E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>3148</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M7" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3155</v>
       </c>
@@ -653,8 +763,22 @@
         <f>((G4+H4)/(G3+H3+G4+H4))*((H3+H4)/(G3+H3+G4+H4))</f>
         <v>0.52140000000000009</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>3155</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3158</v>
       </c>
@@ -675,8 +799,22 @@
         <f>G7+G8</f>
         <v>0.5928000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>3158</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M9" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3177</v>
       </c>
@@ -697,8 +835,22 @@
         <f>(G6-G9)/(1-G9)</f>
         <v>0.68074656188605098</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>3177</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3180</v>
       </c>
@@ -712,8 +864,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>3180</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M11" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10624</v>
       </c>
@@ -727,8 +893,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>10624</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M12" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11045</v>
       </c>
@@ -742,8 +922,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>11045</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M13" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11543</v>
       </c>
@@ -757,8 +951,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>11543</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M14" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11935</v>
       </c>
@@ -772,8 +980,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>11935</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M15" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12433</v>
       </c>
@@ -787,8 +1009,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>12433</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M16" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>12611</v>
       </c>
@@ -802,8 +1038,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>12611</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M17" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>13383</v>
       </c>
@@ -817,8 +1067,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>13383</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M18" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13398</v>
       </c>
@@ -832,8 +1096,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>13398</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M19" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>13479</v>
       </c>
@@ -847,8 +1125,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>13479</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M20" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>13482</v>
       </c>
@@ -862,8 +1154,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>13482</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>13742</v>
       </c>
@@ -877,8 +1183,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>13742</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M22" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>13754</v>
       </c>
@@ -892,8 +1212,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>13754</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M23" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>13932</v>
       </c>
@@ -907,8 +1241,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>13932</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M24" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>14098</v>
       </c>
@@ -922,8 +1270,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>14098</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M25" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>14421</v>
       </c>
@@ -937,8 +1299,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>14421</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M26" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>14454</v>
       </c>
@@ -952,8 +1328,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>14454</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M27" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>14747</v>
       </c>
@@ -967,8 +1357,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>14747</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M28" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>14906</v>
       </c>
@@ -982,8 +1386,22 @@
         <f t="shared" si="0"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>14906</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M29" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>15074</v>
       </c>
@@ -997,8 +1415,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>15074</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M30" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15519</v>
       </c>
@@ -1012,8 +1444,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>15519</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M31" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>15615</v>
       </c>
@@ -1027,8 +1473,22 @@
         <f t="shared" si="0"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>15615</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M32" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>15712</v>
       </c>
@@ -1042,8 +1502,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>15712</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M33" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>15793</v>
       </c>
@@ -1057,8 +1531,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>15793</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M34" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>15878</v>
       </c>
@@ -1072,8 +1560,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>15878</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M35" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>15964</v>
       </c>
@@ -1087,8 +1589,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>15964</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M36" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>16023</v>
       </c>
@@ -1102,8 +1618,22 @@
         <f t="shared" si="0"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>16023</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M37" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>16029</v>
       </c>
@@ -1117,8 +1647,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>16029</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M38" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>16068</v>
       </c>
@@ -1132,8 +1676,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>16068</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M39" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>16142</v>
       </c>
@@ -1147,8 +1705,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>16142</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M40" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>16149</v>
       </c>
@@ -1162,8 +1734,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>16149</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M41" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>16152</v>
       </c>
@@ -1177,8 +1763,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>16152</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M42" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>16171</v>
       </c>
@@ -1192,8 +1792,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>16171</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M43" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>16174</v>
       </c>
@@ -1207,8 +1821,22 @@
         <f t="shared" si="0"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>16174</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M44" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>16557</v>
       </c>
@@ -1222,8 +1850,22 @@
         <f t="shared" si="0"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>16557</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M45" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>16563</v>
       </c>
@@ -1237,8 +1879,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>16563</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M46" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>16587</v>
       </c>
@@ -1252,8 +1908,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>16587</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M47" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>16590</v>
       </c>
@@ -1267,8 +1937,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J48">
+        <v>16590</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M48" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>16602</v>
       </c>
@@ -1282,8 +1966,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J49">
+        <v>16602</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M49" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>16676</v>
       </c>
@@ -1297,8 +1995,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J50">
+        <v>16676</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>16683</v>
       </c>
@@ -1312,8 +2024,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J51">
+        <v>16683</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M51" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>16686</v>
       </c>
@@ -1327,8 +2053,22 @@
         <f t="shared" si="0"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>16686</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M52" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>16705</v>
       </c>
@@ -1342,8 +2082,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J53">
+        <v>16705</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M53" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>16946</v>
       </c>
@@ -1357,8 +2111,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J54">
+        <v>16946</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M54" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>17032</v>
       </c>
@@ -1372,8 +2140,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J55">
+        <v>17032</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M55" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>17039</v>
       </c>
@@ -1387,8 +2169,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J56">
+        <v>17039</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M56" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>17121</v>
       </c>
@@ -1402,8 +2198,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J57">
+        <v>17121</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M57" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>17124</v>
       </c>
@@ -1417,8 +2227,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J58">
+        <v>17124</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M58" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>17136</v>
       </c>
@@ -1432,8 +2256,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J59">
+        <v>17136</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M59" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>17210</v>
       </c>
@@ -1447,8 +2285,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J60">
+        <v>17210</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M60" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>17217</v>
       </c>
@@ -1462,8 +2314,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J61">
+        <v>17217</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M61" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>17220</v>
       </c>
@@ -1477,8 +2343,22 @@
         <f t="shared" si="0"/>
         <v>SAME_0</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J62">
+        <v>17220</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M62" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>17275</v>
       </c>
@@ -1492,8 +2372,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J63">
+        <v>17275</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M63" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>17299</v>
       </c>
@@ -1507,8 +2401,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J64">
+        <v>17299</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M64" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>17314</v>
       </c>
@@ -1522,8 +2430,22 @@
         <f t="shared" si="0"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J65">
+        <v>17314</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M65" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>17388</v>
       </c>
@@ -1537,8 +2459,22 @@
         <f t="shared" si="0"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J66">
+        <v>17388</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M66" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>17447</v>
       </c>
@@ -1549,11 +2485,25 @@
         <v>0</v>
       </c>
       <c r="D67" s="2" t="str">
-        <f t="shared" ref="D67:D101" si="1">IF(B67=0,IF(C67=0,"SAME_0","DIFF_0_1"),IF(C67=1,"SAME_1","DIFF_1_0"))</f>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" ref="D67:D101" si="3">IF(B67=0,IF(C67=0,"SAME_0","DIFF_0_1"),IF(C67=1,"SAME_1","DIFF_1_0"))</f>
+        <v>SAME_0</v>
+      </c>
+      <c r="J67">
+        <v>17447</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67" t="b">
+        <f t="shared" ref="L67:L101" si="4">C67=K67</f>
+        <v>1</v>
+      </c>
+      <c r="M67" t="b">
+        <f t="shared" ref="M67:M101" si="5">B67=K67</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>17803</v>
       </c>
@@ -1564,11 +2514,25 @@
         <v>1</v>
       </c>
       <c r="D68" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J68">
+        <v>17803</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M68" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>18100</v>
       </c>
@@ -1579,11 +2543,25 @@
         <v>0</v>
       </c>
       <c r="D69" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J69">
+        <v>18100</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M69" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>18159</v>
       </c>
@@ -1594,11 +2572,25 @@
         <v>1</v>
       </c>
       <c r="D70" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J70">
+        <v>18159</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M70" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>18189</v>
       </c>
@@ -1609,11 +2601,25 @@
         <v>1</v>
       </c>
       <c r="D71" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J71">
+        <v>18189</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M71" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>18192</v>
       </c>
@@ -1624,11 +2630,25 @@
         <v>0</v>
       </c>
       <c r="D72" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J72">
+        <v>18192</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M72" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>18204</v>
       </c>
@@ -1639,11 +2659,25 @@
         <v>0</v>
       </c>
       <c r="D73" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J73">
+        <v>18204</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M73" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>18278</v>
       </c>
@@ -1654,11 +2688,25 @@
         <v>1</v>
       </c>
       <c r="D74" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J74">
+        <v>18278</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M74" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>18288</v>
       </c>
@@ -1669,11 +2717,25 @@
         <v>1</v>
       </c>
       <c r="D75" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J75">
+        <v>18288</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+      <c r="L75" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M75" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>18521</v>
       </c>
@@ -1684,11 +2746,25 @@
         <v>0</v>
       </c>
       <c r="D76" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J76">
+        <v>18521</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M76" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>18693</v>
       </c>
@@ -1699,11 +2775,25 @@
         <v>0</v>
       </c>
       <c r="D77" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J77">
+        <v>18693</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M77" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>18699</v>
       </c>
@@ -1714,11 +2804,25 @@
         <v>0</v>
       </c>
       <c r="D78" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J78">
+        <v>18699</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M78" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>18723</v>
       </c>
@@ -1729,11 +2833,25 @@
         <v>0</v>
       </c>
       <c r="D79" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J79">
+        <v>18723</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M79" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>18726</v>
       </c>
@@ -1744,11 +2862,25 @@
         <v>1</v>
       </c>
       <c r="D80" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J80">
+        <v>18726</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M80" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>18738</v>
       </c>
@@ -1759,11 +2891,25 @@
         <v>0</v>
       </c>
       <c r="D81" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J81">
+        <v>18738</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M81" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>18812</v>
       </c>
@@ -1774,11 +2920,25 @@
         <v>0</v>
       </c>
       <c r="D82" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J82">
+        <v>18812</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M82" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>18819</v>
       </c>
@@ -1789,11 +2949,25 @@
         <v>0</v>
       </c>
       <c r="D83" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J83">
+        <v>18819</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M83" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>18822</v>
       </c>
@@ -1804,11 +2978,25 @@
         <v>0</v>
       </c>
       <c r="D84" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J84">
+        <v>18822</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M84" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>18997</v>
       </c>
@@ -1819,11 +3007,25 @@
         <v>0</v>
       </c>
       <c r="D85" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J85">
+        <v>18997</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M85" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>19049</v>
       </c>
@@ -1834,11 +3036,25 @@
         <v>0</v>
       </c>
       <c r="D86" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J86">
+        <v>19049</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M86" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>19055</v>
       </c>
@@ -1849,11 +3065,25 @@
         <v>1</v>
       </c>
       <c r="D87" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J87">
+        <v>19055</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+      <c r="L87" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M87" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>19094</v>
       </c>
@@ -1864,11 +3094,25 @@
         <v>1</v>
       </c>
       <c r="D88" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J88">
+        <v>19094</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M88" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>19168</v>
       </c>
@@ -1879,11 +3123,25 @@
         <v>1</v>
       </c>
       <c r="D89" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J89">
+        <v>19168</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M89" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>19178</v>
       </c>
@@ -1894,11 +3152,25 @@
         <v>0</v>
       </c>
       <c r="D90" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J90">
+        <v>19178</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M90" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>19227</v>
       </c>
@@ -1909,11 +3181,25 @@
         <v>0</v>
       </c>
       <c r="D91" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J91">
+        <v>19227</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M91" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>19233</v>
       </c>
@@ -1924,11 +3210,25 @@
         <v>1</v>
       </c>
       <c r="D92" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J92">
+        <v>19233</v>
+      </c>
+      <c r="K92">
+        <v>1</v>
+      </c>
+      <c r="L92" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M92" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>19257</v>
       </c>
@@ -1939,11 +3239,25 @@
         <v>0</v>
       </c>
       <c r="D93" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J93">
+        <v>19257</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M93" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>19583</v>
       </c>
@@ -1954,11 +3268,25 @@
         <v>1</v>
       </c>
       <c r="D94" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J94">
+        <v>19583</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M94" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>19589</v>
       </c>
@@ -1969,11 +3297,25 @@
         <v>1</v>
       </c>
       <c r="D95" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J95">
+        <v>19589</v>
+      </c>
+      <c r="K95">
+        <v>1</v>
+      </c>
+      <c r="L95" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M95" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>19613</v>
       </c>
@@ -1984,11 +3326,25 @@
         <v>1</v>
       </c>
       <c r="D96" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J96">
+        <v>19613</v>
+      </c>
+      <c r="K96">
+        <v>1</v>
+      </c>
+      <c r="L96" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M96" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>19616</v>
       </c>
@@ -1999,11 +3355,25 @@
         <v>0</v>
       </c>
       <c r="D97" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J97">
+        <v>19616</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M97" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>19628</v>
       </c>
@@ -2014,11 +3384,25 @@
         <v>1</v>
       </c>
       <c r="D98" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J98">
+        <v>19628</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M98" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>19702</v>
       </c>
@@ -2029,11 +3413,25 @@
         <v>1</v>
       </c>
       <c r="D99" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SAME_1</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J99">
+        <v>19702</v>
+      </c>
+      <c r="K99">
+        <v>1</v>
+      </c>
+      <c r="L99" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M99" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>19712</v>
       </c>
@@ -2044,11 +3442,25 @@
         <v>1</v>
       </c>
       <c r="D100" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>DIFF_0_1</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J100">
+        <v>19712</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M100" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>19731</v>
       </c>
@@ -2059,8 +3471,32 @@
         <v>0</v>
       </c>
       <c r="D101" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SAME_0</v>
+        <f t="shared" si="3"/>
+        <v>SAME_0</v>
+      </c>
+      <c r="J101">
+        <v>19731</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M101" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L102">
+        <f>COUNTIF(L2:L101,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="M102">
+        <f>COUNTIF(M2:M101,FALSE)</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>